<commit_message>
Changes made on 6/8/2019
</commit_message>
<xml_diff>
--- a/Data/AppData.xlsx
+++ b/Data/AppData.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7FD1F9-6FE7-4D77-86DD-43BE3818CA7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA1C908-4ED2-4EB4-B8E9-895206F0B12E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EntradaData" sheetId="1" r:id="rId1"/>
+    <sheet name="Capabilities" sheetId="2" r:id="rId2"/>
+    <sheet name="Data1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Firstname</t>
   </si>
@@ -113,13 +115,67 @@
   </si>
   <si>
     <t>China</t>
+  </si>
+  <si>
+    <t>devicename</t>
+  </si>
+  <si>
+    <t>98897a433352455332</t>
+  </si>
+  <si>
+    <t>platformname</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>platformVersion</t>
+  </si>
+  <si>
+    <t>appPackage</t>
+  </si>
+  <si>
+    <t>appActivity</t>
+  </si>
+  <si>
+    <t>com.entradahealth.entrada.android</t>
+  </si>
+  <si>
+    <t>com.entradahealth.entrada.android.app.personal.activities.user_select.UserSelectActivity</t>
+  </si>
+  <si>
+    <t>automationName</t>
+  </si>
+  <si>
+    <t>uiautomator2</t>
+  </si>
+  <si>
+    <t>Capability_name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>full-reset</t>
+  </si>
+  <si>
+    <t>a1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Entrada@1</t>
+  </si>
+  <si>
+    <t>deviceName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,8 +183,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +202,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,14 +221,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -574,4 +654,125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3080E906-50A2-4471-9ECB-D95A6E073D49}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2BA043D-1980-4EB0-82E0-7306BB8EAA93}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{D6FA9EB6-FBA9-4849-894E-E9324CB61885}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{24875103-D7BA-4837-835B-1C19BC1917E5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>